<commit_message>
Updated weeks and milestones
See title.
</commit_message>
<xml_diff>
--- a/Documents/SynchoSchedule.xlsx
+++ b/Documents/SynchoSchedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Week</t>
   </si>
@@ -25,6 +25,18 @@
   </si>
   <si>
     <t>Milestones</t>
+  </si>
+  <si>
+    <t>Wrap up for final presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Project Manager: 1.Jake 2.Colton: Make sure people know what they’re doing.  Come up with weekly sprint objectives.  Have a rough timeline done.                                                                                               • Responsive web developer team: 1. Kimberly 2.Jared 3. Alex: start rough draft website, start looking at angular JS.                                                                                                                                                                       • Central webserver/DB developers: 1.Alex 2.Jared 3.Kimberly: rough layout for DB and start reading • Android App Developers: 1.Colton 2.Jake: Get software ready, start reading.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Get server up and running, Basic App running on an android device. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website pull and push from DB and app pull and push from DB. </t>
   </si>
 </sst>
 </file>
@@ -95,16 +107,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,135 +432,144 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.7109375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A2" s="4">
+    <row r="2" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>42403</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A3" s="5">
+      <c r="B2" s="4">
+        <v>42408</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
-        <v>42410</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A4" s="4">
+      <c r="B3" s="7">
+        <v>42415</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
-        <v>42417</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A5" s="5">
+      <c r="B4" s="4">
+        <v>42423</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
-        <v>42424</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A6" s="4">
+      <c r="B5" s="7">
+        <v>42429</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>42431</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A7" s="5">
+      <c r="B6" s="4">
+        <v>42436</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
-        <v>42438</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A8" s="4">
+      <c r="B7" s="7">
+        <v>42443</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
-        <v>42445</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A9" s="5">
+      <c r="B8" s="4">
+        <v>42450</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
-        <v>42452</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A10" s="4">
+      <c r="B9" s="7">
+        <v>42457</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
-        <v>42459</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A11" s="5">
+      <c r="B10" s="4">
+        <v>42464</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
-        <v>42466</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A12" s="4">
+      <c r="B11" s="7">
+        <v>42471</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="7">
-        <v>42473</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="50.1" customHeight="1">
-      <c r="A13" s="5">
+      <c r="B12" s="4">
+        <v>42478</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="99.95" customHeight="1">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
-        <v>42480</v>
-      </c>
-      <c r="C13" s="2"/>
+      <c r="B13" s="7">
+        <v>42485</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>